<commit_message>
atualiza readme, referencias extras, e deixa link para pacotes
</commit_message>
<xml_diff>
--- a/referencias_extras.xlsx
+++ b/referencias_extras.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>aula</t>
   </si>
@@ -67,6 +67,40 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>https://bookdown.org/yihui/rmarkdown/xaringan.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Escrita científica</t>
+  </si>
+  <si>
+    <t>Writing Reproducible Research Papers with R Markdown</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://resulumit.com/teaching/rmd_workshop.html#1</t>
+    </r>
+  </si>
+  <si>
+    <t>RMarkdown</t>
+  </si>
+  <si>
+    <t>R Markdown Cheatsheet</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://www.rstudio.com/wp-content/uploads/2015/02/rmarkdown-cheatsheet.pdf</t>
     </r>
   </si>
 </sst>
@@ -1488,18 +1522,34 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>13</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>16</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
@@ -1844,6 +1894,8 @@
     <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="http://slides.yihui.name/xaringan/"/>
     <hyperlink ref="D3" r:id="rId2" location="" tooltip="" display="https://github.com/yihui/xaringan/wiki"/>
     <hyperlink ref="D4" r:id="rId3" location="" tooltip="" display="https://bookdown.org/yihui/rmarkdown/xaringan.html"/>
+    <hyperlink ref="D5" r:id="rId4" location="" tooltip="" display="https://resulumit.com/teaching/rmd_workshop.html#1"/>
+    <hyperlink ref="D6" r:id="rId5" location="" tooltip="" display="https://www.rstudio.com/wp-content/uploads/2015/02/rmarkdown-cheatsheet.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>